<commit_message>
Se incluye función de descargar informe
</commit_message>
<xml_diff>
--- a/Auto-Informes/plantillas/archivo.xlsx
+++ b/Auto-Informes/plantillas/archivo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pipe-\Documents\Miniproyectos_Python\Auto-Informes\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A40F06A8-97AD-46F3-A6D8-09D13A2A4D96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{186715EB-E4CC-4AAB-BA65-0928868DEB26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25215" yWindow="2085" windowWidth="15375" windowHeight="7875" xr2:uid="{3F6BE4C7-7E6F-4C19-960C-25384A0D0FB4}"/>
   </bookViews>
@@ -54,9 +54,6 @@
     <t>vendedor</t>
   </si>
   <si>
-    <t>region</t>
-  </si>
-  <si>
     <t>Norte</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>Nevera</t>
+  </si>
+  <si>
+    <t>región</t>
   </si>
 </sst>
 </file>
@@ -455,7 +455,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -480,7 +480,7 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
         <v>45301</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>100</v>
@@ -501,10 +501,10 @@
         <v>900000</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -512,7 +512,7 @@
         <v>45413</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>10</v>
@@ -525,10 +525,10 @@
         <v>850000</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -536,7 +536,7 @@
         <v>45516</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>90</v>
@@ -549,10 +549,10 @@
         <v>963000</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -560,7 +560,7 @@
         <v>45569</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>20</v>
@@ -573,10 +573,10 @@
         <v>741000</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -584,23 +584,23 @@
         <v>41267</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>100</v>
       </c>
       <c r="D6">
-        <f t="shared" ref="D3:D6" si="0">E6/100</f>
+        <f t="shared" ref="D6" si="0">E6/100</f>
         <v>3510</v>
       </c>
       <c r="E6">
         <v>351000</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>